<commit_message>
Emissions ceramics + update notebook residential tertiary
</commit_message>
<xml_diff>
--- a/Models/Prospective_conso/data/Hypotheses_ceramics_1D.xlsx
+++ b/Models/Prospective_conso/data/Hypotheses_ceramics_1D.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engie-my.sharepoint.com/personal/kv6345_engie_com/Documents/Documents/5-Python/Energy-Alternatives-Planing/Models/Prospective_conso/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ADB03513-176D-44AA-88BF-06AD4B39A1D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{ADB03513-176D-44AA-88BF-06AD4B39A1D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1C9D44F-E1D8-4852-9E72-0B964919CCEA}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{263B99EF-50CC-433E-9045-94D7F8818570}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11325" activeTab="3" xr2:uid="{263B99EF-50CC-433E-9045-94D7F8818570}"/>
   </bookViews>
   <sheets>
     <sheet name="0D" sheetId="1" r:id="rId1"/>
     <sheet name="Production_system" sheetId="2" r:id="rId2"/>
     <sheet name="Production_system_year" sheetId="3" r:id="rId3"/>
-    <sheet name="retrofit_Transition" sheetId="4" r:id="rId4"/>
+    <sheet name="year_Vecteur" sheetId="5" r:id="rId4"/>
+    <sheet name="retrofit_Transition" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="33">
   <si>
     <t>Nom</t>
   </si>
@@ -113,6 +114,30 @@
   </si>
   <si>
     <t>Séchoir thermique + RC + Four biomasse</t>
+  </si>
+  <si>
+    <t>Vecteur</t>
+  </si>
+  <si>
+    <t>direct_emissions</t>
+  </si>
+  <si>
+    <t>indirect_emissions</t>
+  </si>
+  <si>
+    <t>elec</t>
+  </si>
+  <si>
+    <t>gaz</t>
+  </si>
+  <si>
+    <t>fioul</t>
+  </si>
+  <si>
+    <t>bois</t>
+  </si>
+  <si>
+    <t>charbon</t>
   </si>
 </sst>
 </file>
@@ -503,7 +528,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,7 +705,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,10 +1157,111 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCDE4F52-1213-4E96-AFE3-14D53043F5A9}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2">
+        <v>2020</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>2020</v>
+      </c>
+      <c r="C3">
+        <v>187</v>
+      </c>
+      <c r="D3">
+        <f>227-C3</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>2020</v>
+      </c>
+      <c r="C4">
+        <v>272</v>
+      </c>
+      <c r="D4">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>2020</v>
+      </c>
+      <c r="C5">
+        <v>27</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>2020</v>
+      </c>
+      <c r="C6">
+        <v>346.5</v>
+      </c>
+      <c r="D6">
+        <v>28.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F969234-B378-4A56-A622-56267A5202AB}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
new food and beverages input file + updates input files industry
</commit_message>
<xml_diff>
--- a/Models/Prospective_conso/data/Hypotheses_ceramics_1D.xlsx
+++ b/Models/Prospective_conso/data/Hypotheses_ceramics_1D.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engie-my.sharepoint.com/personal/kv6345_engie_com/Documents/Documents/5-Python/Energy-Alternatives-Planing/Models/Prospective_conso/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="6_{9E90345F-21AA-41F4-AB6B-6E5ACC4EF9AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="6_{9E90345F-21AA-41F4-AB6B-6E5ACC4EF9AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04CB8CF3-8D19-4C10-B808-F756636B7EDC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{263B99EF-50CC-433E-9045-94D7F8818570}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{263B99EF-50CC-433E-9045-94D7F8818570}"/>
   </bookViews>
   <sheets>
     <sheet name="0D" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="34">
   <si>
     <t>Nom</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>init_energy_need_per_unite_prod</t>
+  </si>
+  <si>
+    <t>seasonal_efficiency</t>
   </si>
 </sst>
 </file>
@@ -173,7 +176,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -196,45 +199,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -554,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529A1527-08E9-4208-98F7-539760163740}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -565,10 +541,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -576,39 +552,39 @@
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>270.88069255578102</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>2020</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>2050</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>69.95</v>
       </c>
     </row>
@@ -616,7 +592,7 @@
       <c r="A7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>0.1</v>
       </c>
     </row>
@@ -631,7 +607,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -641,82 +617,82 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>16530.162694442846</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>1394.1101067602399</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>181.05326061821299</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>0</v>
       </c>
     </row>
@@ -731,7 +707,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection sqref="A1:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -741,7 +717,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -761,182 +737,182 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>0.29591836734693877</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>1.5764924839957177</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>0.24525708985651209</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>0.52687074829931979</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>1.5379999999999998</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>1.8518518518518517E-3</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>0.29591836734693877</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>1.5764924839957177</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>0.24525708985651207</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>1.5850092764378478</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>0.15849248399571764</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>0.24525708985651209</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>1.8159616573902289</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>0.12</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>1.8518518518518517E-3</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>1.5850092764378478</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>0.15849248399571764</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>0.24525708985651207</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>0.29591836734693877</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>0.15849248399571764</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>0.24525708985651209</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>1.3634615384615383</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>0.52687074829931979</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>0.12</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>1.8518518518518517E-3</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>1.3634615384615383</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>0.29591836734693877</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>0.15849248399571764</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>0.24525708985651207</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>1.3634615384615383</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>0</v>
       </c>
     </row>
@@ -948,10 +924,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCDE4F52-1213-4E96-AFE3-14D53043F5A9}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -959,89 +935,192 @@
     <col min="3" max="4" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B2">
-        <v>2020</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B2" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>45</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.6052170689771601</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B3">
-        <v>2020</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C3" s="2">
         <v>187</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <f>227-C3</f>
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="E3" s="2">
+        <v>0.551103804343124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B4">
-        <v>2020</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C4" s="2">
         <v>272</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>57</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="E4" s="2">
+        <v>0.51435851685912504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B5">
-        <v>2020</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C5" s="2">
         <v>27</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.5662422623604989</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B6">
-        <v>2020</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C6" s="2">
         <v>346.5</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>28.5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.57180540919810341</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>15</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.65542394009027061</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C8" s="2">
+        <v>44</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.63931085679287936</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C9" s="2">
+        <v>272</v>
+      </c>
+      <c r="D9" s="2">
+        <v>57</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.5843585168591251</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C10" s="2">
+        <v>27</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.70341918284350091</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C11" s="2">
+        <v>346.5</v>
+      </c>
+      <c r="D11" s="2">
+        <v>28.5</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.6742595810037435</v>
       </c>
     </row>
   </sheetData>
@@ -1054,8 +1133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F969234-B378-4A56-A622-56267A5202AB}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1065,352 +1144,352 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="1">
         <v>2020</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
         <v>0.44143516213614781</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>0.34033390206830183</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
+      <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
         <v>2.8372734488755363E-2</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2">
         <v>0.10720568223306448</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="2">
         <v>8.2652519073730432E-2</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="1">
         <v>2020</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
         <v>0.76670317634173046</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
         <v>4.7097480832420588E-2</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
         <v>0.18619934282584885</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="1">
         <v>2020</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
         <v>0.80221562630385412</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
         <v>2.9605787366382718E-3</v>
       </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
         <v>0.19482379495950747</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="1">
         <v>2020</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
         <v>0.31988733996889729</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
         <v>0.60242573461008475</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
         <v>7.7686925421017905E-2</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B6" s="1">
         <v>2020</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
         <v>1</v>
       </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="1">
         <v>2020</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
         <v>0.75402015849811499</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
         <v>6.2860660152342845E-2</v>
       </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2">
         <v>0.18311918134954222</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="1">
         <v>2020</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
         <v>0.57575757575757569</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="2">
         <v>0.42424242424242425</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="1">
         <v>2020</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
         <v>1</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="1">
         <v>2020</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ajout de fichiers html amélioration de la doc
</commit_message>
<xml_diff>
--- a/Models/Prospective_conso/data/Hypotheses_ceramics_1D.xlsx
+++ b/Models/Prospective_conso/data/Hypotheses_ceramics_1D.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engie-my.sharepoint.com/personal/kv6345_engie_com/Documents/Documents/5-Python/Energy-Alternatives-Planing/Models/Prospective_conso/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robin.girard/Documents/Code/Etude/Energy-Alternatives-Planing/Models/Prospective_conso/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="6_{9E90345F-21AA-41F4-AB6B-6E5ACC4EF9AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{04CB8CF3-8D19-4C10-B808-F756636B7EDC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54CD02F-C32E-4547-8BE3-E1E81C291B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{263B99EF-50CC-433E-9045-94D7F8818570}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" activeTab="3" xr2:uid="{263B99EF-50CC-433E-9045-94D7F8818570}"/>
   </bookViews>
   <sheets>
     <sheet name="0D" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -232,7 +230,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -534,13 +532,13 @@
       <selection sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="46.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -548,7 +546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
@@ -556,7 +554,7 @@
         <v>270.88069255578102</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -564,7 +562,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -572,7 +570,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -580,7 +578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
@@ -588,7 +586,7 @@
         <v>69.95</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>30</v>
       </c>
@@ -610,13 +608,13 @@
       <selection sqref="A1:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -624,7 +622,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -632,7 +630,7 @@
         <v>16530.162694442846</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -640,7 +638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -648,7 +646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -656,7 +654,7 @@
         <v>1394.1101067602399</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -664,7 +662,7 @@
         <v>181.05326061821299</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -672,7 +670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -680,7 +678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -688,7 +686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -710,13 +708,13 @@
       <selection sqref="A1:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
     <col min="2" max="6" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -736,7 +734,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -756,7 +754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -776,7 +774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -796,7 +794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -816,7 +814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -836,7 +834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -856,7 +854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -876,7 +874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -896,7 +894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -926,16 +924,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCDE4F52-1213-4E96-AFE3-14D53043F5A9}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="4" width="15.109375" customWidth="1"/>
+    <col min="3" max="4" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -952,7 +950,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -969,7 +967,7 @@
         <v>0.6052170689771601</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -987,7 +985,7 @@
         <v>0.551103804343124</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
@@ -1004,7 +1002,7 @@
         <v>0.51435851685912504</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
@@ -1021,7 +1019,7 @@
         <v>0.5662422623604989</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
@@ -1038,12 +1036,12 @@
         <v>0.57180540919810341</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="2">
-        <v>2020</v>
+        <v>2050</v>
       </c>
       <c r="C7" s="2">
         <v>0</v>
@@ -1055,12 +1053,12 @@
         <v>0.65542394009027061</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="2">
-        <v>2020</v>
+        <v>2050</v>
       </c>
       <c r="C8" s="2">
         <v>44</v>
@@ -1072,12 +1070,12 @@
         <v>0.63931085679287936</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="2">
-        <v>2020</v>
+        <v>2050</v>
       </c>
       <c r="C9" s="2">
         <v>272</v>
@@ -1089,12 +1087,12 @@
         <v>0.5843585168591251</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="2">
-        <v>2020</v>
+        <v>2050</v>
       </c>
       <c r="C10" s="2">
         <v>27</v>
@@ -1106,12 +1104,12 @@
         <v>0.70341918284350091</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="2">
-        <v>2020</v>
+        <v>2050</v>
       </c>
       <c r="C11" s="2">
         <v>346.5</v>
@@ -1133,17 +1131,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F969234-B378-4A56-A622-56267A5202AB}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -1178,7 +1176,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
@@ -1213,7 +1211,7 @@
         <v>8.2652519073730432E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1248,7 +1246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1283,7 +1281,7 @@
         <v>0.19482379495950747</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -1318,7 +1316,7 @@
         <v>7.7686925421017905E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
@@ -1353,7 +1351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -1388,7 +1386,7 @@
         <v>0.18311918134954222</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>18</v>
       </c>
@@ -1423,7 +1421,7 @@
         <v>0.42424242424242425</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -1458,7 +1456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>

</xml_diff>